<commit_message>
tabela de preços atualizada em 16/12/2023
</commit_message>
<xml_diff>
--- a/orcamento/valores_exames_samvida.xlsx
+++ b/orcamento/valores_exames_samvida.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="719" uniqueCount="719">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="718" uniqueCount="718">
   <si>
     <t>Local</t>
   </si>
@@ -901,9 +901,6 @@
   </si>
   <si>
     <t xml:space="preserve">PESQUISA DE AUTO-ANTICORPOS ANTICELULA (FAN)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PESQUISA DE FUNGOS</t>
   </si>
   <si>
     <t xml:space="preserve">PESQUISA DE SANGUE OCULTO NAS FEZES</t>
@@ -2781,7 +2778,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetViews>
-    <sheetView topLeftCell="A280" zoomScale="100" workbookViewId="0">
+    <sheetView topLeftCell="A289" zoomScale="100" workbookViewId="0">
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -6045,7 +6042,7 @@
         <v>296</v>
       </c>
       <c r="C296" s="8">
-        <v>19000</v>
+        <v>15</v>
       </c>
     </row>
     <row r="297" ht="14.25">
@@ -6056,7 +6053,7 @@
         <v>297</v>
       </c>
       <c r="C297" s="8">
-        <v>15</v>
+        <v>30</v>
       </c>
     </row>
     <row r="298" ht="14.25">
@@ -6067,7 +6064,7 @@
         <v>298</v>
       </c>
       <c r="C298" s="8">
-        <v>30</v>
+        <v>10</v>
       </c>
     </row>
     <row r="299" ht="14.25">
@@ -6083,24 +6080,24 @@
     </row>
     <row r="300" ht="14.25">
       <c r="A300" s="1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B300" s="7" t="s">
         <v>300</v>
       </c>
       <c r="C300" s="8">
-        <v>10</v>
+        <v>16</v>
       </c>
     </row>
     <row r="301" ht="14.25">
       <c r="A301" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B301" s="7" t="s">
         <v>301</v>
       </c>
       <c r="C301" s="8">
-        <v>16</v>
+        <v>50</v>
       </c>
     </row>
     <row r="302" ht="14.25">
@@ -6111,7 +6108,7 @@
         <v>302</v>
       </c>
       <c r="C302" s="8">
-        <v>50</v>
+        <v>6</v>
       </c>
     </row>
     <row r="303" ht="14.25">
@@ -6122,7 +6119,7 @@
         <v>303</v>
       </c>
       <c r="C303" s="8">
-        <v>6</v>
+        <v>14</v>
       </c>
     </row>
     <row r="304" ht="14.25">
@@ -6133,7 +6130,7 @@
         <v>304</v>
       </c>
       <c r="C304" s="8">
-        <v>14</v>
+        <v>10.18</v>
       </c>
     </row>
     <row r="305" ht="14.25">
@@ -6155,7 +6152,7 @@
         <v>306</v>
       </c>
       <c r="C306" s="8">
-        <v>10.18</v>
+        <v>25</v>
       </c>
     </row>
     <row r="307" ht="14.25">
@@ -6177,7 +6174,7 @@
         <v>308</v>
       </c>
       <c r="C308" s="8">
-        <v>25</v>
+        <v>10</v>
       </c>
     </row>
     <row r="309" ht="14.25">
@@ -6188,7 +6185,7 @@
         <v>309</v>
       </c>
       <c r="C309" s="8">
-        <v>10</v>
+        <v>6.4699999999999998</v>
       </c>
     </row>
     <row r="310" ht="14.25">
@@ -6199,7 +6196,7 @@
         <v>310</v>
       </c>
       <c r="C310" s="8">
-        <v>6.4699999999999998</v>
+        <v>10</v>
       </c>
     </row>
     <row r="311" ht="14.25">
@@ -6210,7 +6207,7 @@
         <v>311</v>
       </c>
       <c r="C311" s="8">
-        <v>10</v>
+        <v>20</v>
       </c>
     </row>
     <row r="312" ht="14.25">
@@ -6232,7 +6229,7 @@
         <v>313</v>
       </c>
       <c r="C313" s="8">
-        <v>20</v>
+        <v>15.5</v>
       </c>
     </row>
     <row r="314" ht="14.25">
@@ -6243,7 +6240,7 @@
         <v>314</v>
       </c>
       <c r="C314" s="8">
-        <v>15.5</v>
+        <v>55</v>
       </c>
     </row>
     <row r="315" ht="14.25">
@@ -6254,18 +6251,18 @@
         <v>315</v>
       </c>
       <c r="C315" s="8">
-        <v>55</v>
+        <v>20</v>
       </c>
     </row>
     <row r="316" ht="14.25">
       <c r="A316" s="1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B316" s="7" t="s">
         <v>316</v>
       </c>
       <c r="C316" s="8">
-        <v>20</v>
+        <v>556</v>
       </c>
     </row>
     <row r="317" ht="14.25">
@@ -6276,7 +6273,7 @@
         <v>317</v>
       </c>
       <c r="C317" s="8">
-        <v>556</v>
+        <v>506</v>
       </c>
     </row>
     <row r="318" ht="14.25">
@@ -6287,7 +6284,7 @@
         <v>318</v>
       </c>
       <c r="C318" s="8">
-        <v>506</v>
+        <v>656</v>
       </c>
     </row>
     <row r="319" ht="14.25">
@@ -6298,7 +6295,7 @@
         <v>319</v>
       </c>
       <c r="C319" s="8">
-        <v>656</v>
+        <v>906</v>
       </c>
     </row>
     <row r="320" ht="14.25">
@@ -6309,7 +6306,7 @@
         <v>320</v>
       </c>
       <c r="C320" s="8">
-        <v>906</v>
+        <v>1006</v>
       </c>
     </row>
     <row r="321" ht="14.25">
@@ -6320,7 +6317,7 @@
         <v>321</v>
       </c>
       <c r="C321" s="8">
-        <v>1006</v>
+        <v>466</v>
       </c>
     </row>
     <row r="322" ht="14.25">
@@ -6331,7 +6328,7 @@
         <v>322</v>
       </c>
       <c r="C322" s="8">
-        <v>466</v>
+        <v>611</v>
       </c>
     </row>
     <row r="323" ht="14.25">
@@ -6342,7 +6339,7 @@
         <v>323</v>
       </c>
       <c r="C323" s="8">
-        <v>611</v>
+        <v>466</v>
       </c>
     </row>
     <row r="324" ht="14.25">
@@ -6353,7 +6350,7 @@
         <v>324</v>
       </c>
       <c r="C324" s="8">
-        <v>466</v>
+        <v>611</v>
       </c>
     </row>
     <row r="325" ht="14.25">
@@ -6364,7 +6361,7 @@
         <v>325</v>
       </c>
       <c r="C325" s="8">
-        <v>611</v>
+        <v>466</v>
       </c>
     </row>
     <row r="326" ht="14.25">
@@ -6386,7 +6383,7 @@
         <v>327</v>
       </c>
       <c r="C327" s="8">
-        <v>466</v>
+        <v>611</v>
       </c>
     </row>
     <row r="328" ht="14.25">
@@ -6419,7 +6416,7 @@
         <v>330</v>
       </c>
       <c r="C330" s="8">
-        <v>611</v>
+        <v>466</v>
       </c>
     </row>
     <row r="331" ht="14.25">
@@ -6441,7 +6438,7 @@
         <v>332</v>
       </c>
       <c r="C332" s="8">
-        <v>466</v>
+        <v>611</v>
       </c>
     </row>
     <row r="333" ht="14.25">
@@ -6452,7 +6449,7 @@
         <v>333</v>
       </c>
       <c r="C333" s="8">
-        <v>611</v>
+        <v>466</v>
       </c>
     </row>
     <row r="334" ht="14.25">
@@ -6481,11 +6478,11 @@
       <c r="A336" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B336" s="7" t="s">
+      <c r="B336" s="9" t="s">
         <v>336</v>
       </c>
-      <c r="C336" s="8">
-        <v>466</v>
+      <c r="C336" s="10">
+        <v>611</v>
       </c>
     </row>
     <row r="337" ht="14.25">
@@ -6496,7 +6493,7 @@
         <v>337</v>
       </c>
       <c r="C337" s="10">
-        <v>611</v>
+        <v>466</v>
       </c>
     </row>
     <row r="338" ht="14.25">
@@ -6507,7 +6504,7 @@
         <v>338</v>
       </c>
       <c r="C338" s="10">
-        <v>466</v>
+        <v>611</v>
       </c>
     </row>
     <row r="339" ht="14.25">
@@ -6518,7 +6515,7 @@
         <v>339</v>
       </c>
       <c r="C339" s="10">
-        <v>611</v>
+        <v>466</v>
       </c>
     </row>
     <row r="340" ht="14.25">
@@ -6529,7 +6526,7 @@
         <v>340</v>
       </c>
       <c r="C340" s="10">
-        <v>466</v>
+        <v>611</v>
       </c>
     </row>
     <row r="341" ht="14.25">
@@ -6540,7 +6537,7 @@
         <v>341</v>
       </c>
       <c r="C341" s="10">
-        <v>611</v>
+        <v>466</v>
       </c>
     </row>
     <row r="342" ht="14.25">
@@ -6562,7 +6559,7 @@
         <v>343</v>
       </c>
       <c r="C343" s="10">
-        <v>466</v>
+        <v>611</v>
       </c>
     </row>
     <row r="344" ht="14.25">
@@ -6584,7 +6581,7 @@
         <v>345</v>
       </c>
       <c r="C345" s="10">
-        <v>611</v>
+        <v>466</v>
       </c>
     </row>
     <row r="346" ht="14.25">
@@ -6595,7 +6592,7 @@
         <v>346</v>
       </c>
       <c r="C346" s="10">
-        <v>466</v>
+        <v>611</v>
       </c>
     </row>
     <row r="347" ht="14.25">
@@ -6606,7 +6603,7 @@
         <v>347</v>
       </c>
       <c r="C347" s="10">
-        <v>611</v>
+        <v>466</v>
       </c>
     </row>
     <row r="348" ht="14.25">
@@ -6617,7 +6614,7 @@
         <v>348</v>
       </c>
       <c r="C348" s="10">
-        <v>466</v>
+        <v>611</v>
       </c>
     </row>
     <row r="349" ht="14.25">
@@ -6628,7 +6625,7 @@
         <v>349</v>
       </c>
       <c r="C349" s="10">
-        <v>611</v>
+        <v>466</v>
       </c>
     </row>
     <row r="350" ht="14.25">
@@ -6639,7 +6636,7 @@
         <v>350</v>
       </c>
       <c r="C350" s="10">
-        <v>466</v>
+        <v>611</v>
       </c>
     </row>
     <row r="351" ht="14.25">
@@ -6650,7 +6647,7 @@
         <v>351</v>
       </c>
       <c r="C351" s="10">
-        <v>611</v>
+        <v>466</v>
       </c>
     </row>
     <row r="352" ht="14.25">
@@ -6672,7 +6669,7 @@
         <v>353</v>
       </c>
       <c r="C353" s="10">
-        <v>466</v>
+        <v>611</v>
       </c>
     </row>
     <row r="354" ht="14.25">
@@ -6683,7 +6680,7 @@
         <v>354</v>
       </c>
       <c r="C354" s="10">
-        <v>611</v>
+        <v>466</v>
       </c>
     </row>
     <row r="355" ht="14.25">
@@ -6694,7 +6691,7 @@
         <v>355</v>
       </c>
       <c r="C355" s="10">
-        <v>466</v>
+        <v>611</v>
       </c>
     </row>
     <row r="356" ht="14.25">
@@ -6705,7 +6702,7 @@
         <v>356</v>
       </c>
       <c r="C356" s="10">
-        <v>611</v>
+        <v>466</v>
       </c>
     </row>
     <row r="357" ht="14.25">
@@ -6716,7 +6713,7 @@
         <v>357</v>
       </c>
       <c r="C357" s="10">
-        <v>466</v>
+        <v>611</v>
       </c>
     </row>
     <row r="358" ht="14.25">
@@ -6727,7 +6724,7 @@
         <v>358</v>
       </c>
       <c r="C358" s="10">
-        <v>611</v>
+        <v>466</v>
       </c>
     </row>
     <row r="359" ht="14.25">
@@ -6738,7 +6735,7 @@
         <v>359</v>
       </c>
       <c r="C359" s="10">
-        <v>466</v>
+        <v>611</v>
       </c>
     </row>
     <row r="360" ht="14.25">
@@ -6749,7 +6746,7 @@
         <v>360</v>
       </c>
       <c r="C360" s="10">
-        <v>611</v>
+        <v>466</v>
       </c>
     </row>
     <row r="361" ht="14.25">
@@ -6760,7 +6757,7 @@
         <v>361</v>
       </c>
       <c r="C361" s="10">
-        <v>466</v>
+        <v>611</v>
       </c>
     </row>
     <row r="362" ht="14.25">
@@ -6771,7 +6768,7 @@
         <v>362</v>
       </c>
       <c r="C362" s="10">
-        <v>611</v>
+        <v>466</v>
       </c>
     </row>
     <row r="363" ht="14.25">
@@ -6782,7 +6779,7 @@
         <v>363</v>
       </c>
       <c r="C363" s="10">
-        <v>466</v>
+        <v>611</v>
       </c>
     </row>
     <row r="364" ht="14.25">
@@ -6793,7 +6790,7 @@
         <v>364</v>
       </c>
       <c r="C364" s="10">
-        <v>611</v>
+        <v>466</v>
       </c>
     </row>
     <row r="365" ht="14.25">
@@ -6804,7 +6801,7 @@
         <v>365</v>
       </c>
       <c r="C365" s="10">
-        <v>466</v>
+        <v>611</v>
       </c>
     </row>
     <row r="366" ht="14.25">
@@ -6815,7 +6812,7 @@
         <v>366</v>
       </c>
       <c r="C366" s="10">
-        <v>611</v>
+        <v>466</v>
       </c>
     </row>
     <row r="367" ht="14.25">
@@ -6826,7 +6823,7 @@
         <v>367</v>
       </c>
       <c r="C367" s="10">
-        <v>466</v>
+        <v>611</v>
       </c>
     </row>
     <row r="368" ht="14.25">
@@ -6837,7 +6834,7 @@
         <v>368</v>
       </c>
       <c r="C368" s="10">
-        <v>611</v>
+        <v>466</v>
       </c>
     </row>
     <row r="369" ht="14.25">
@@ -6848,7 +6845,7 @@
         <v>369</v>
       </c>
       <c r="C369" s="10">
-        <v>466</v>
+        <v>611</v>
       </c>
     </row>
     <row r="370" ht="14.25">
@@ -6859,7 +6856,7 @@
         <v>370</v>
       </c>
       <c r="C370" s="10">
-        <v>611</v>
+        <v>466</v>
       </c>
     </row>
     <row r="371" ht="14.25">
@@ -6870,7 +6867,7 @@
         <v>371</v>
       </c>
       <c r="C371" s="10">
-        <v>466</v>
+        <v>611</v>
       </c>
     </row>
     <row r="372" ht="14.25">
@@ -6881,7 +6878,7 @@
         <v>372</v>
       </c>
       <c r="C372" s="10">
-        <v>611</v>
+        <v>466</v>
       </c>
     </row>
     <row r="373" ht="14.25">
@@ -6892,7 +6889,7 @@
         <v>373</v>
       </c>
       <c r="C373" s="10">
-        <v>466</v>
+        <v>611</v>
       </c>
     </row>
     <row r="374" ht="14.25">
@@ -6903,7 +6900,7 @@
         <v>374</v>
       </c>
       <c r="C374" s="10">
-        <v>611</v>
+        <v>466</v>
       </c>
     </row>
     <row r="375" ht="14.25">
@@ -6914,7 +6911,7 @@
         <v>375</v>
       </c>
       <c r="C375" s="10">
-        <v>466</v>
+        <v>611</v>
       </c>
     </row>
     <row r="376" ht="14.25">
@@ -6925,7 +6922,7 @@
         <v>376</v>
       </c>
       <c r="C376" s="10">
-        <v>611</v>
+        <v>466</v>
       </c>
     </row>
     <row r="377" ht="14.25">
@@ -6980,7 +6977,7 @@
         <v>381</v>
       </c>
       <c r="C381" s="10">
-        <v>466</v>
+        <v>611</v>
       </c>
     </row>
     <row r="382" ht="14.25">
@@ -6991,7 +6988,7 @@
         <v>382</v>
       </c>
       <c r="C382" s="10">
-        <v>611</v>
+        <v>466</v>
       </c>
     </row>
     <row r="383" ht="14.25">
@@ -7002,7 +6999,7 @@
         <v>383</v>
       </c>
       <c r="C383" s="10">
-        <v>466</v>
+        <v>611</v>
       </c>
     </row>
     <row r="384" ht="14.25">
@@ -7013,7 +7010,7 @@
         <v>384</v>
       </c>
       <c r="C384" s="10">
-        <v>611</v>
+        <v>466</v>
       </c>
     </row>
     <row r="385" ht="14.25">
@@ -7024,7 +7021,7 @@
         <v>385</v>
       </c>
       <c r="C385" s="10">
-        <v>466</v>
+        <v>486</v>
       </c>
     </row>
     <row r="386" ht="14.25">
@@ -7035,7 +7032,7 @@
         <v>386</v>
       </c>
       <c r="C386" s="10">
-        <v>486</v>
+        <v>611</v>
       </c>
     </row>
     <row r="387" ht="14.25">
@@ -7046,7 +7043,7 @@
         <v>387</v>
       </c>
       <c r="C387" s="10">
-        <v>611</v>
+        <v>466</v>
       </c>
     </row>
     <row r="388" ht="14.25">
@@ -7057,7 +7054,7 @@
         <v>388</v>
       </c>
       <c r="C388" s="10">
-        <v>466</v>
+        <v>486</v>
       </c>
     </row>
     <row r="389" ht="14.25">
@@ -7068,7 +7065,7 @@
         <v>389</v>
       </c>
       <c r="C389" s="10">
-        <v>486</v>
+        <v>611</v>
       </c>
     </row>
     <row r="390" ht="14.25">
@@ -7079,7 +7076,7 @@
         <v>390</v>
       </c>
       <c r="C390" s="10">
-        <v>611</v>
+        <v>866</v>
       </c>
     </row>
     <row r="391" ht="14.25">
@@ -7101,7 +7098,7 @@
         <v>392</v>
       </c>
       <c r="C392" s="10">
-        <v>866</v>
+        <v>466</v>
       </c>
     </row>
     <row r="393" ht="14.25">
@@ -7112,7 +7109,7 @@
         <v>393</v>
       </c>
       <c r="C393" s="10">
-        <v>466</v>
+        <v>611</v>
       </c>
     </row>
     <row r="394" ht="14.25">
@@ -7123,7 +7120,7 @@
         <v>394</v>
       </c>
       <c r="C394" s="10">
-        <v>611</v>
+        <v>466</v>
       </c>
     </row>
     <row r="395" ht="14.25">
@@ -7134,7 +7131,7 @@
         <v>395</v>
       </c>
       <c r="C395" s="10">
-        <v>466</v>
+        <v>611</v>
       </c>
     </row>
     <row r="396" ht="14.25">
@@ -7145,7 +7142,7 @@
         <v>396</v>
       </c>
       <c r="C396" s="10">
-        <v>611</v>
+        <v>466</v>
       </c>
     </row>
     <row r="397" ht="14.25">
@@ -7156,7 +7153,7 @@
         <v>397</v>
       </c>
       <c r="C397" s="10">
-        <v>466</v>
+        <v>611</v>
       </c>
     </row>
     <row r="398" ht="14.25">
@@ -7167,7 +7164,7 @@
         <v>398</v>
       </c>
       <c r="C398" s="10">
-        <v>611</v>
+        <v>466</v>
       </c>
     </row>
     <row r="399" ht="14.25">
@@ -7189,7 +7186,7 @@
         <v>400</v>
       </c>
       <c r="C400" s="10">
-        <v>466</v>
+        <v>611</v>
       </c>
     </row>
     <row r="401" ht="14.25">
@@ -7200,7 +7197,7 @@
         <v>401</v>
       </c>
       <c r="C401" s="10">
-        <v>611</v>
+        <v>466</v>
       </c>
     </row>
     <row r="402" ht="14.25">
@@ -7211,7 +7208,7 @@
         <v>402</v>
       </c>
       <c r="C402" s="10">
-        <v>466</v>
+        <v>611</v>
       </c>
     </row>
     <row r="403" ht="14.25">
@@ -7222,7 +7219,7 @@
         <v>403</v>
       </c>
       <c r="C403" s="10">
-        <v>611</v>
+        <v>466</v>
       </c>
     </row>
     <row r="404" ht="14.25">
@@ -7233,7 +7230,7 @@
         <v>404</v>
       </c>
       <c r="C404" s="10">
-        <v>466</v>
+        <v>611</v>
       </c>
     </row>
     <row r="405" ht="14.25">
@@ -7244,7 +7241,7 @@
         <v>405</v>
       </c>
       <c r="C405" s="10">
-        <v>611</v>
+        <v>466</v>
       </c>
     </row>
     <row r="406" ht="14.25">
@@ -7255,7 +7252,7 @@
         <v>406</v>
       </c>
       <c r="C406" s="10">
-        <v>466</v>
+        <v>611</v>
       </c>
     </row>
     <row r="407" ht="14.25">
@@ -7266,7 +7263,7 @@
         <v>407</v>
       </c>
       <c r="C407" s="10">
-        <v>611</v>
+        <v>466</v>
       </c>
     </row>
     <row r="408" ht="14.25">
@@ -7277,7 +7274,7 @@
         <v>408</v>
       </c>
       <c r="C408" s="10">
-        <v>466</v>
+        <v>611</v>
       </c>
     </row>
     <row r="409" ht="14.25">
@@ -7288,7 +7285,7 @@
         <v>409</v>
       </c>
       <c r="C409" s="10">
-        <v>611</v>
+        <v>466</v>
       </c>
     </row>
     <row r="410" ht="14.25">
@@ -7299,7 +7296,7 @@
         <v>410</v>
       </c>
       <c r="C410" s="10">
-        <v>466</v>
+        <v>611</v>
       </c>
     </row>
     <row r="411" ht="14.25">
@@ -7310,7 +7307,7 @@
         <v>411</v>
       </c>
       <c r="C411" s="10">
-        <v>611</v>
+        <v>466</v>
       </c>
     </row>
     <row r="412" ht="14.25">
@@ -7321,7 +7318,7 @@
         <v>412</v>
       </c>
       <c r="C412" s="10">
-        <v>466</v>
+        <v>611</v>
       </c>
     </row>
     <row r="413" ht="14.25">
@@ -7332,7 +7329,7 @@
         <v>413</v>
       </c>
       <c r="C413" s="10">
-        <v>611</v>
+        <v>466</v>
       </c>
     </row>
     <row r="414" ht="14.25">
@@ -7343,7 +7340,7 @@
         <v>414</v>
       </c>
       <c r="C414" s="10">
-        <v>466</v>
+        <v>611</v>
       </c>
     </row>
     <row r="415" ht="14.25">
@@ -7354,7 +7351,7 @@
         <v>415</v>
       </c>
       <c r="C415" s="10">
-        <v>611</v>
+        <v>466</v>
       </c>
     </row>
     <row r="416" ht="14.25">
@@ -7365,7 +7362,7 @@
         <v>416</v>
       </c>
       <c r="C416" s="10">
-        <v>466</v>
+        <v>611</v>
       </c>
     </row>
     <row r="417" ht="14.25">
@@ -7376,7 +7373,7 @@
         <v>417</v>
       </c>
       <c r="C417" s="10">
-        <v>611</v>
+        <v>466</v>
       </c>
     </row>
     <row r="418" ht="14.25">
@@ -7387,7 +7384,7 @@
         <v>418</v>
       </c>
       <c r="C418" s="10">
-        <v>466</v>
+        <v>611</v>
       </c>
     </row>
     <row r="419" ht="14.25">
@@ -7398,7 +7395,7 @@
         <v>419</v>
       </c>
       <c r="C419" s="10">
-        <v>611</v>
+        <v>466</v>
       </c>
     </row>
     <row r="420" ht="14.25">
@@ -7409,7 +7406,7 @@
         <v>420</v>
       </c>
       <c r="C420" s="10">
-        <v>466</v>
+        <v>611</v>
       </c>
     </row>
     <row r="421" ht="14.25">
@@ -7420,7 +7417,7 @@
         <v>421</v>
       </c>
       <c r="C421" s="10">
-        <v>611</v>
+        <v>466</v>
       </c>
     </row>
     <row r="422" ht="14.25">
@@ -7431,7 +7428,7 @@
         <v>422</v>
       </c>
       <c r="C422" s="10">
-        <v>466</v>
+        <v>611</v>
       </c>
     </row>
     <row r="423" ht="14.25">
@@ -7442,7 +7439,7 @@
         <v>423</v>
       </c>
       <c r="C423" s="10">
-        <v>611</v>
+        <v>466</v>
       </c>
     </row>
     <row r="424" ht="14.25">
@@ -7464,7 +7461,7 @@
         <v>425</v>
       </c>
       <c r="C425" s="10">
-        <v>466</v>
+        <v>611</v>
       </c>
     </row>
     <row r="426" ht="14.25">
@@ -7486,7 +7483,7 @@
         <v>427</v>
       </c>
       <c r="C427" s="10">
-        <v>611</v>
+        <v>466</v>
       </c>
     </row>
     <row r="428" ht="14.25">
@@ -7497,7 +7494,7 @@
         <v>428</v>
       </c>
       <c r="C428" s="10">
-        <v>466</v>
+        <v>611</v>
       </c>
     </row>
     <row r="429" ht="14.25">
@@ -7508,7 +7505,7 @@
         <v>429</v>
       </c>
       <c r="C429" s="10">
-        <v>611</v>
+        <v>466</v>
       </c>
     </row>
     <row r="430" ht="14.25">
@@ -7519,7 +7516,7 @@
         <v>430</v>
       </c>
       <c r="C430" s="10">
-        <v>466</v>
+        <v>611</v>
       </c>
     </row>
     <row r="431" ht="14.25">
@@ -7530,7 +7527,7 @@
         <v>431</v>
       </c>
       <c r="C431" s="10">
-        <v>611</v>
+        <v>466</v>
       </c>
     </row>
     <row r="432" ht="14.25">
@@ -7541,7 +7538,7 @@
         <v>432</v>
       </c>
       <c r="C432" s="10">
-        <v>466</v>
+        <v>611</v>
       </c>
     </row>
     <row r="433" ht="14.25">
@@ -7552,7 +7549,7 @@
         <v>433</v>
       </c>
       <c r="C433" s="10">
-        <v>611</v>
+        <v>466</v>
       </c>
     </row>
     <row r="434" ht="14.25">
@@ -7563,7 +7560,7 @@
         <v>434</v>
       </c>
       <c r="C434" s="10">
-        <v>466</v>
+        <v>611</v>
       </c>
     </row>
     <row r="435" ht="14.25">
@@ -7596,7 +7593,7 @@
         <v>437</v>
       </c>
       <c r="C437" s="10">
-        <v>611</v>
+        <v>466</v>
       </c>
     </row>
     <row r="438" ht="14.25">
@@ -7629,7 +7626,7 @@
         <v>440</v>
       </c>
       <c r="C440" s="10">
-        <v>466</v>
+        <v>611</v>
       </c>
     </row>
     <row r="441" ht="14.25">
@@ -7640,7 +7637,7 @@
         <v>441</v>
       </c>
       <c r="C441" s="10">
-        <v>611</v>
+        <v>466</v>
       </c>
     </row>
     <row r="442" ht="14.25">
@@ -7651,7 +7648,7 @@
         <v>442</v>
       </c>
       <c r="C442" s="10">
-        <v>466</v>
+        <v>611</v>
       </c>
     </row>
     <row r="443" ht="14.25">
@@ -7662,7 +7659,7 @@
         <v>443</v>
       </c>
       <c r="C443" s="10">
-        <v>611</v>
+        <v>466</v>
       </c>
     </row>
     <row r="444" ht="14.25">
@@ -7673,7 +7670,7 @@
         <v>444</v>
       </c>
       <c r="C444" s="10">
-        <v>466</v>
+        <v>611</v>
       </c>
     </row>
     <row r="445" ht="14.25">
@@ -7684,7 +7681,7 @@
         <v>445</v>
       </c>
       <c r="C445" s="10">
-        <v>611</v>
+        <v>466</v>
       </c>
     </row>
     <row r="446" ht="14.25">
@@ -7695,7 +7692,7 @@
         <v>446</v>
       </c>
       <c r="C446" s="10">
-        <v>466</v>
+        <v>611</v>
       </c>
     </row>
     <row r="447" ht="14.25">
@@ -7706,7 +7703,7 @@
         <v>447</v>
       </c>
       <c r="C447" s="10">
-        <v>611</v>
+        <v>466</v>
       </c>
     </row>
     <row r="448" ht="14.25">
@@ -7717,7 +7714,7 @@
         <v>448</v>
       </c>
       <c r="C448" s="10">
-        <v>466</v>
+        <v>611</v>
       </c>
     </row>
     <row r="449" ht="14.25">
@@ -7728,7 +7725,7 @@
         <v>449</v>
       </c>
       <c r="C449" s="10">
-        <v>611</v>
+        <v>506</v>
       </c>
     </row>
     <row r="450" ht="14.25">
@@ -7739,7 +7736,7 @@
         <v>450</v>
       </c>
       <c r="C450" s="10">
-        <v>506</v>
+        <v>611</v>
       </c>
     </row>
     <row r="451" ht="14.25">
@@ -7750,7 +7747,7 @@
         <v>451</v>
       </c>
       <c r="C451" s="10">
-        <v>611</v>
+        <v>466</v>
       </c>
     </row>
     <row r="452" ht="14.25">
@@ -7761,7 +7758,7 @@
         <v>452</v>
       </c>
       <c r="C452" s="10">
-        <v>466</v>
+        <v>611</v>
       </c>
     </row>
     <row r="453" ht="14.25">
@@ -7772,7 +7769,7 @@
         <v>453</v>
       </c>
       <c r="C453" s="10">
-        <v>611</v>
+        <v>466</v>
       </c>
     </row>
     <row r="454" ht="14.25">
@@ -7783,7 +7780,7 @@
         <v>454</v>
       </c>
       <c r="C454" s="10">
-        <v>466</v>
+        <v>611</v>
       </c>
     </row>
     <row r="455" ht="14.25">
@@ -7794,18 +7791,18 @@
         <v>455</v>
       </c>
       <c r="C455" s="10">
-        <v>611</v>
+        <v>466</v>
       </c>
     </row>
     <row r="456" ht="14.25">
       <c r="A456" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B456" s="9" t="s">
         <v>456</v>
       </c>
       <c r="C456" s="10">
-        <v>466</v>
+        <v>24</v>
       </c>
     </row>
     <row r="457" ht="14.25">
@@ -7816,7 +7813,7 @@
         <v>457</v>
       </c>
       <c r="C457" s="10">
-        <v>24</v>
+        <v>30</v>
       </c>
     </row>
     <row r="458" ht="14.25">
@@ -7827,18 +7824,18 @@
         <v>458</v>
       </c>
       <c r="C458" s="10">
-        <v>30</v>
+        <v>40</v>
       </c>
     </row>
     <row r="459" ht="14.25">
       <c r="A459" s="1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B459" s="9" t="s">
         <v>459</v>
       </c>
       <c r="C459" s="10">
-        <v>40</v>
+        <v>56</v>
       </c>
     </row>
     <row r="460" ht="14.25">
@@ -8212,7 +8209,7 @@
         <v>493</v>
       </c>
       <c r="C493" s="10">
-        <v>56</v>
+        <v>156</v>
       </c>
     </row>
     <row r="494" ht="14.25">
@@ -8223,7 +8220,7 @@
         <v>494</v>
       </c>
       <c r="C494" s="10">
-        <v>156</v>
+        <v>56</v>
       </c>
     </row>
     <row r="495" ht="14.25">
@@ -8333,7 +8330,7 @@
         <v>504</v>
       </c>
       <c r="C504" s="10">
-        <v>56</v>
+        <v>126</v>
       </c>
     </row>
     <row r="505" ht="14.25">
@@ -8344,7 +8341,7 @@
         <v>505</v>
       </c>
       <c r="C505" s="10">
-        <v>126</v>
+        <v>156</v>
       </c>
     </row>
     <row r="506" ht="14.25">
@@ -8355,7 +8352,7 @@
         <v>506</v>
       </c>
       <c r="C506" s="10">
-        <v>156</v>
+        <v>56</v>
       </c>
     </row>
     <row r="507" ht="14.25">
@@ -8366,7 +8363,7 @@
         <v>507</v>
       </c>
       <c r="C507" s="10">
-        <v>56</v>
+        <v>21</v>
       </c>
     </row>
     <row r="508" ht="14.25">
@@ -8421,7 +8418,7 @@
         <v>512</v>
       </c>
       <c r="C512" s="10">
-        <v>21</v>
+        <v>56</v>
       </c>
     </row>
     <row r="513" ht="14.25">
@@ -8575,7 +8572,7 @@
         <v>526</v>
       </c>
       <c r="C526" s="10">
-        <v>56</v>
+        <v>156</v>
       </c>
     </row>
     <row r="527" ht="14.25">
@@ -8597,7 +8594,7 @@
         <v>528</v>
       </c>
       <c r="C528" s="10">
-        <v>156</v>
+        <v>56</v>
       </c>
     </row>
     <row r="529" ht="14.25">
@@ -8822,13 +8819,13 @@
     </row>
     <row r="549" ht="14.25">
       <c r="A549" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B549" s="9" t="s">
         <v>549</v>
       </c>
       <c r="C549" s="10">
-        <v>56</v>
+        <v>15</v>
       </c>
     </row>
     <row r="550" ht="14.25">
@@ -8839,7 +8836,7 @@
         <v>550</v>
       </c>
       <c r="C550" s="10">
-        <v>15</v>
+        <v>10</v>
       </c>
     </row>
     <row r="551" ht="14.25">
@@ -8850,7 +8847,7 @@
         <v>551</v>
       </c>
       <c r="C551" s="10">
-        <v>10</v>
+        <v>38</v>
       </c>
     </row>
     <row r="552" ht="14.25">
@@ -8861,7 +8858,7 @@
         <v>552</v>
       </c>
       <c r="C552" s="10">
-        <v>38</v>
+        <v>66</v>
       </c>
     </row>
     <row r="553" ht="14.25">
@@ -8872,7 +8869,7 @@
         <v>553</v>
       </c>
       <c r="C553" s="10">
-        <v>66</v>
+        <v>89</v>
       </c>
     </row>
     <row r="554" ht="14.25">
@@ -8883,7 +8880,7 @@
         <v>554</v>
       </c>
       <c r="C554" s="10">
-        <v>89</v>
+        <v>30</v>
       </c>
     </row>
     <row r="555" ht="14.25">
@@ -8894,7 +8891,7 @@
         <v>555</v>
       </c>
       <c r="C555" s="10">
-        <v>30</v>
+        <v>13</v>
       </c>
     </row>
     <row r="556" ht="14.25">
@@ -8905,7 +8902,7 @@
         <v>556</v>
       </c>
       <c r="C556" s="10">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="557" ht="14.25">
@@ -8916,7 +8913,7 @@
         <v>557</v>
       </c>
       <c r="C557" s="10">
-        <v>15</v>
+        <v>6</v>
       </c>
     </row>
     <row r="558" ht="14.25">
@@ -8927,7 +8924,7 @@
         <v>558</v>
       </c>
       <c r="C558" s="10">
-        <v>6</v>
+        <v>28</v>
       </c>
     </row>
     <row r="559" ht="14.25">
@@ -8938,7 +8935,7 @@
         <v>559</v>
       </c>
       <c r="C559" s="10">
-        <v>28</v>
+        <v>59</v>
       </c>
     </row>
     <row r="560" ht="14.25">
@@ -8949,7 +8946,7 @@
         <v>560</v>
       </c>
       <c r="C560" s="10">
-        <v>59</v>
+        <v>30</v>
       </c>
     </row>
     <row r="561" ht="14.25">
@@ -8960,7 +8957,7 @@
         <v>561</v>
       </c>
       <c r="C561" s="10">
-        <v>30</v>
+        <v>11</v>
       </c>
     </row>
     <row r="562" ht="14.25">
@@ -8971,7 +8968,7 @@
         <v>562</v>
       </c>
       <c r="C562" s="10">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="563" ht="14.25">
@@ -8982,18 +8979,18 @@
         <v>563</v>
       </c>
       <c r="C563" s="10">
-        <v>9</v>
+        <v>30</v>
       </c>
     </row>
     <row r="564" ht="14.25">
       <c r="A564" s="1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B564" s="9" t="s">
         <v>564</v>
       </c>
       <c r="C564" s="10">
-        <v>30</v>
+        <v>406</v>
       </c>
     </row>
     <row r="565" ht="14.25">
@@ -9004,7 +9001,7 @@
         <v>565</v>
       </c>
       <c r="C565" s="10">
-        <v>406</v>
+        <v>476</v>
       </c>
     </row>
     <row r="566" ht="14.25">
@@ -9026,7 +9023,7 @@
         <v>567</v>
       </c>
       <c r="C567" s="10">
-        <v>476</v>
+        <v>556</v>
       </c>
     </row>
     <row r="568" ht="14.25">
@@ -9037,7 +9034,7 @@
         <v>568</v>
       </c>
       <c r="C568" s="10">
-        <v>556</v>
+        <v>271</v>
       </c>
     </row>
     <row r="569" ht="14.25">
@@ -9059,7 +9056,7 @@
         <v>570</v>
       </c>
       <c r="C570" s="10">
-        <v>271</v>
+        <v>356</v>
       </c>
     </row>
     <row r="571" ht="14.25">
@@ -9081,7 +9078,7 @@
         <v>572</v>
       </c>
       <c r="C572" s="10">
-        <v>356</v>
+        <v>476</v>
       </c>
     </row>
     <row r="573" ht="14.25">
@@ -9092,7 +9089,7 @@
         <v>573</v>
       </c>
       <c r="C573" s="10">
-        <v>476</v>
+        <v>271</v>
       </c>
     </row>
     <row r="574" ht="14.25">
@@ -9147,7 +9144,7 @@
         <v>578</v>
       </c>
       <c r="C578" s="10">
-        <v>271</v>
+        <v>356</v>
       </c>
     </row>
     <row r="579" ht="14.25">
@@ -9158,7 +9155,7 @@
         <v>579</v>
       </c>
       <c r="C579" s="10">
-        <v>356</v>
+        <v>271</v>
       </c>
     </row>
     <row r="580" ht="14.25">
@@ -9169,7 +9166,7 @@
         <v>580</v>
       </c>
       <c r="C580" s="10">
-        <v>271</v>
+        <v>356</v>
       </c>
     </row>
     <row r="581" ht="14.25">
@@ -9180,7 +9177,7 @@
         <v>581</v>
       </c>
       <c r="C581" s="10">
-        <v>356</v>
+        <v>271</v>
       </c>
     </row>
     <row r="582" ht="14.25">
@@ -9191,7 +9188,7 @@
         <v>582</v>
       </c>
       <c r="C582" s="10">
-        <v>271</v>
+        <v>356</v>
       </c>
     </row>
     <row r="583" ht="14.25">
@@ -9202,7 +9199,7 @@
         <v>583</v>
       </c>
       <c r="C583" s="10">
-        <v>356</v>
+        <v>271</v>
       </c>
     </row>
     <row r="584" ht="14.25">
@@ -9213,7 +9210,7 @@
         <v>584</v>
       </c>
       <c r="C584" s="10">
-        <v>271</v>
+        <v>356</v>
       </c>
     </row>
     <row r="585" ht="14.25">
@@ -9224,7 +9221,7 @@
         <v>585</v>
       </c>
       <c r="C585" s="10">
-        <v>356</v>
+        <v>271</v>
       </c>
     </row>
     <row r="586" ht="14.25">
@@ -9235,7 +9232,7 @@
         <v>586</v>
       </c>
       <c r="C586" s="10">
-        <v>271</v>
+        <v>356</v>
       </c>
     </row>
     <row r="587" ht="14.25">
@@ -9246,7 +9243,7 @@
         <v>587</v>
       </c>
       <c r="C587" s="10">
-        <v>356</v>
+        <v>46</v>
       </c>
     </row>
     <row r="588" ht="14.25">
@@ -9257,7 +9254,7 @@
         <v>588</v>
       </c>
       <c r="C588" s="10">
-        <v>46</v>
+        <v>271</v>
       </c>
     </row>
     <row r="589" ht="14.25">
@@ -9268,7 +9265,7 @@
         <v>589</v>
       </c>
       <c r="C589" s="10">
-        <v>271</v>
+        <v>356</v>
       </c>
     </row>
     <row r="590" ht="14.25">
@@ -9279,7 +9276,7 @@
         <v>590</v>
       </c>
       <c r="C590" s="10">
-        <v>356</v>
+        <v>271</v>
       </c>
     </row>
     <row r="591" ht="14.25">
@@ -9290,7 +9287,7 @@
         <v>591</v>
       </c>
       <c r="C591" s="10">
-        <v>271</v>
+        <v>356</v>
       </c>
     </row>
     <row r="592" ht="14.25">
@@ -9301,7 +9298,7 @@
         <v>592</v>
       </c>
       <c r="C592" s="10">
-        <v>356</v>
+        <v>271</v>
       </c>
     </row>
     <row r="593" ht="14.25">
@@ -9312,7 +9309,7 @@
         <v>593</v>
       </c>
       <c r="C593" s="10">
-        <v>271</v>
+        <v>356</v>
       </c>
     </row>
     <row r="594" ht="14.25">
@@ -9323,7 +9320,7 @@
         <v>594</v>
       </c>
       <c r="C594" s="10">
-        <v>356</v>
+        <v>271</v>
       </c>
     </row>
     <row r="595" ht="14.25">
@@ -9334,7 +9331,7 @@
         <v>595</v>
       </c>
       <c r="C595" s="10">
-        <v>271</v>
+        <v>356</v>
       </c>
     </row>
     <row r="596" ht="14.25">
@@ -9345,7 +9342,7 @@
         <v>596</v>
       </c>
       <c r="C596" s="10">
-        <v>356</v>
+        <v>271</v>
       </c>
     </row>
     <row r="597" ht="14.25">
@@ -9356,7 +9353,7 @@
         <v>597</v>
       </c>
       <c r="C597" s="10">
-        <v>271</v>
+        <v>356</v>
       </c>
     </row>
     <row r="598" ht="14.25">
@@ -9367,7 +9364,7 @@
         <v>598</v>
       </c>
       <c r="C598" s="10">
-        <v>356</v>
+        <v>271</v>
       </c>
     </row>
     <row r="599" ht="14.25">
@@ -9378,7 +9375,7 @@
         <v>599</v>
       </c>
       <c r="C599" s="10">
-        <v>271</v>
+        <v>356</v>
       </c>
     </row>
     <row r="600" ht="14.25">
@@ -9389,7 +9386,7 @@
         <v>600</v>
       </c>
       <c r="C600" s="10">
-        <v>356</v>
+        <v>271</v>
       </c>
     </row>
     <row r="601" ht="14.25">
@@ -9400,7 +9397,7 @@
         <v>601</v>
       </c>
       <c r="C601" s="10">
-        <v>271</v>
+        <v>356</v>
       </c>
     </row>
     <row r="602" ht="14.25">
@@ -9411,7 +9408,7 @@
         <v>602</v>
       </c>
       <c r="C602" s="10">
-        <v>356</v>
+        <v>271</v>
       </c>
     </row>
     <row r="603" ht="14.25">
@@ -9422,7 +9419,7 @@
         <v>603</v>
       </c>
       <c r="C603" s="10">
-        <v>271</v>
+        <v>356</v>
       </c>
     </row>
     <row r="604" ht="14.25">
@@ -9444,7 +9441,7 @@
         <v>605</v>
       </c>
       <c r="C605" s="10">
-        <v>356</v>
+        <v>271</v>
       </c>
     </row>
     <row r="606" ht="14.25">
@@ -9466,7 +9463,7 @@
         <v>607</v>
       </c>
       <c r="C607" s="10">
-        <v>271</v>
+        <v>356</v>
       </c>
     </row>
     <row r="608" ht="14.25">
@@ -9477,7 +9474,7 @@
         <v>608</v>
       </c>
       <c r="C608" s="10">
-        <v>356</v>
+        <v>271</v>
       </c>
     </row>
     <row r="609" ht="14.25">
@@ -9488,7 +9485,7 @@
         <v>609</v>
       </c>
       <c r="C609" s="10">
-        <v>271</v>
+        <v>356</v>
       </c>
     </row>
     <row r="610" ht="14.25">
@@ -9499,7 +9496,7 @@
         <v>610</v>
       </c>
       <c r="C610" s="10">
-        <v>356</v>
+        <v>271</v>
       </c>
     </row>
     <row r="611" ht="14.25">
@@ -9521,7 +9518,7 @@
         <v>612</v>
       </c>
       <c r="C612" s="10">
-        <v>271</v>
+        <v>356</v>
       </c>
     </row>
     <row r="613" ht="14.25">
@@ -9532,7 +9529,7 @@
         <v>613</v>
       </c>
       <c r="C613" s="10">
-        <v>356</v>
+        <v>271</v>
       </c>
     </row>
     <row r="614" ht="14.25">
@@ -9543,7 +9540,7 @@
         <v>614</v>
       </c>
       <c r="C614" s="10">
-        <v>271</v>
+        <v>356</v>
       </c>
     </row>
     <row r="615" ht="14.25">
@@ -9554,7 +9551,7 @@
         <v>615</v>
       </c>
       <c r="C615" s="10">
-        <v>356</v>
+        <v>271</v>
       </c>
     </row>
     <row r="616" ht="14.25">
@@ -9565,7 +9562,7 @@
         <v>616</v>
       </c>
       <c r="C616" s="10">
-        <v>271</v>
+        <v>356</v>
       </c>
     </row>
     <row r="617" ht="14.25">
@@ -9576,7 +9573,7 @@
         <v>617</v>
       </c>
       <c r="C617" s="10">
-        <v>356</v>
+        <v>271</v>
       </c>
     </row>
     <row r="618" ht="14.25">
@@ -9587,7 +9584,7 @@
         <v>618</v>
       </c>
       <c r="C618" s="10">
-        <v>271</v>
+        <v>356</v>
       </c>
     </row>
     <row r="619" ht="14.25">
@@ -9598,7 +9595,7 @@
         <v>619</v>
       </c>
       <c r="C619" s="10">
-        <v>356</v>
+        <v>271</v>
       </c>
     </row>
     <row r="620" ht="14.25">
@@ -9609,7 +9606,7 @@
         <v>620</v>
       </c>
       <c r="C620" s="10">
-        <v>271</v>
+        <v>356</v>
       </c>
     </row>
     <row r="621" ht="14.25">
@@ -9620,7 +9617,7 @@
         <v>621</v>
       </c>
       <c r="C621" s="10">
-        <v>356</v>
+        <v>271</v>
       </c>
     </row>
     <row r="622" ht="14.25">
@@ -9631,7 +9628,7 @@
         <v>622</v>
       </c>
       <c r="C622" s="10">
-        <v>271</v>
+        <v>356</v>
       </c>
     </row>
     <row r="623" ht="14.25">
@@ -9642,7 +9639,7 @@
         <v>623</v>
       </c>
       <c r="C623" s="10">
-        <v>356</v>
+        <v>271</v>
       </c>
     </row>
     <row r="624" ht="14.25">
@@ -9653,7 +9650,7 @@
         <v>624</v>
       </c>
       <c r="C624" s="10">
-        <v>271</v>
+        <v>356</v>
       </c>
     </row>
     <row r="625" ht="14.25">
@@ -9664,7 +9661,7 @@
         <v>625</v>
       </c>
       <c r="C625" s="10">
-        <v>356</v>
+        <v>271</v>
       </c>
     </row>
     <row r="626" ht="14.25">
@@ -9675,7 +9672,7 @@
         <v>626</v>
       </c>
       <c r="C626" s="10">
-        <v>271</v>
+        <v>356</v>
       </c>
     </row>
     <row r="627" ht="14.25">
@@ -9686,7 +9683,7 @@
         <v>627</v>
       </c>
       <c r="C627" s="10">
-        <v>356</v>
+        <v>271</v>
       </c>
     </row>
     <row r="628" ht="14.25">
@@ -9697,7 +9694,7 @@
         <v>628</v>
       </c>
       <c r="C628" s="10">
-        <v>271</v>
+        <v>456</v>
       </c>
     </row>
     <row r="629" ht="14.25">
@@ -9708,7 +9705,7 @@
         <v>629</v>
       </c>
       <c r="C629" s="10">
-        <v>456</v>
+        <v>271</v>
       </c>
     </row>
     <row r="630" ht="14.25">
@@ -9719,7 +9716,7 @@
         <v>630</v>
       </c>
       <c r="C630" s="10">
-        <v>271</v>
+        <v>356</v>
       </c>
     </row>
     <row r="631" ht="14.25">
@@ -9730,7 +9727,7 @@
         <v>631</v>
       </c>
       <c r="C631" s="10">
-        <v>356</v>
+        <v>271</v>
       </c>
     </row>
     <row r="632" ht="14.25">
@@ -9741,7 +9738,7 @@
         <v>632</v>
       </c>
       <c r="C632" s="10">
-        <v>271</v>
+        <v>356</v>
       </c>
     </row>
     <row r="633" ht="14.25">
@@ -9752,7 +9749,7 @@
         <v>633</v>
       </c>
       <c r="C633" s="10">
-        <v>356</v>
+        <v>271</v>
       </c>
     </row>
     <row r="634" ht="14.25">
@@ -9763,7 +9760,7 @@
         <v>634</v>
       </c>
       <c r="C634" s="10">
-        <v>271</v>
+        <v>356</v>
       </c>
     </row>
     <row r="635" ht="14.25">
@@ -9774,7 +9771,7 @@
         <v>635</v>
       </c>
       <c r="C635" s="10">
-        <v>356</v>
+        <v>271</v>
       </c>
     </row>
     <row r="636" ht="14.25">
@@ -9785,7 +9782,7 @@
         <v>636</v>
       </c>
       <c r="C636" s="10">
-        <v>271</v>
+        <v>356</v>
       </c>
     </row>
     <row r="637" ht="14.25">
@@ -9796,7 +9793,7 @@
         <v>637</v>
       </c>
       <c r="C637" s="10">
-        <v>356</v>
+        <v>271</v>
       </c>
     </row>
     <row r="638" ht="14.25">
@@ -9807,7 +9804,7 @@
         <v>638</v>
       </c>
       <c r="C638" s="10">
-        <v>271</v>
+        <v>356</v>
       </c>
     </row>
     <row r="639" ht="14.25">
@@ -9818,7 +9815,7 @@
         <v>639</v>
       </c>
       <c r="C639" s="10">
-        <v>356</v>
+        <v>271</v>
       </c>
     </row>
     <row r="640" ht="14.25">
@@ -9829,7 +9826,7 @@
         <v>640</v>
       </c>
       <c r="C640" s="10">
-        <v>271</v>
+        <v>356</v>
       </c>
     </row>
     <row r="641" ht="14.25">
@@ -9840,7 +9837,7 @@
         <v>641</v>
       </c>
       <c r="C641" s="10">
-        <v>356</v>
+        <v>271</v>
       </c>
     </row>
     <row r="642" ht="14.25">
@@ -9851,7 +9848,7 @@
         <v>642</v>
       </c>
       <c r="C642" s="10">
-        <v>271</v>
+        <v>356</v>
       </c>
     </row>
     <row r="643" ht="14.25">
@@ -9862,7 +9859,7 @@
         <v>643</v>
       </c>
       <c r="C643" s="10">
-        <v>356</v>
+        <v>271</v>
       </c>
     </row>
     <row r="644" ht="14.25">
@@ -9873,7 +9870,7 @@
         <v>644</v>
       </c>
       <c r="C644" s="10">
-        <v>271</v>
+        <v>356</v>
       </c>
     </row>
     <row r="645" ht="14.25">
@@ -9884,7 +9881,7 @@
         <v>645</v>
       </c>
       <c r="C645" s="10">
-        <v>356</v>
+        <v>271</v>
       </c>
     </row>
     <row r="646" ht="14.25">
@@ -9895,7 +9892,7 @@
         <v>646</v>
       </c>
       <c r="C646" s="10">
-        <v>271</v>
+        <v>356</v>
       </c>
     </row>
     <row r="647" ht="14.25">
@@ -9906,7 +9903,7 @@
         <v>647</v>
       </c>
       <c r="C647" s="10">
-        <v>356</v>
+        <v>271</v>
       </c>
     </row>
     <row r="648" ht="14.25">
@@ -9917,7 +9914,7 @@
         <v>648</v>
       </c>
       <c r="C648" s="10">
-        <v>271</v>
+        <v>356</v>
       </c>
     </row>
     <row r="649" ht="14.25">
@@ -9928,7 +9925,7 @@
         <v>649</v>
       </c>
       <c r="C649" s="10">
-        <v>356</v>
+        <v>271</v>
       </c>
     </row>
     <row r="650" ht="14.25">
@@ -9939,7 +9936,7 @@
         <v>650</v>
       </c>
       <c r="C650" s="10">
-        <v>271</v>
+        <v>356</v>
       </c>
     </row>
     <row r="651" ht="14.25">
@@ -9950,7 +9947,7 @@
         <v>651</v>
       </c>
       <c r="C651" s="10">
-        <v>356</v>
+        <v>271</v>
       </c>
     </row>
     <row r="652" ht="14.25">
@@ -9961,7 +9958,7 @@
         <v>652</v>
       </c>
       <c r="C652" s="10">
-        <v>271</v>
+        <v>356</v>
       </c>
     </row>
     <row r="653" ht="14.25">
@@ -9983,7 +9980,7 @@
         <v>654</v>
       </c>
       <c r="C654" s="10">
-        <v>356</v>
+        <v>456</v>
       </c>
     </row>
     <row r="655" ht="14.25">
@@ -9994,7 +9991,7 @@
         <v>655</v>
       </c>
       <c r="C655" s="10">
-        <v>456</v>
+        <v>271</v>
       </c>
     </row>
     <row r="656" ht="14.25">
@@ -10005,7 +10002,7 @@
         <v>656</v>
       </c>
       <c r="C656" s="10">
-        <v>271</v>
+        <v>356</v>
       </c>
     </row>
     <row r="657" ht="14.25">
@@ -10016,7 +10013,7 @@
         <v>657</v>
       </c>
       <c r="C657" s="10">
-        <v>356</v>
+        <v>271</v>
       </c>
     </row>
     <row r="658" ht="14.25">
@@ -10027,7 +10024,7 @@
         <v>658</v>
       </c>
       <c r="C658" s="10">
-        <v>271</v>
+        <v>356</v>
       </c>
     </row>
     <row r="659" ht="14.25">
@@ -10038,7 +10035,7 @@
         <v>659</v>
       </c>
       <c r="C659" s="10">
-        <v>356</v>
+        <v>271</v>
       </c>
     </row>
     <row r="660" ht="14.25">
@@ -10054,13 +10051,13 @@
     </row>
     <row r="661" ht="14.25">
       <c r="A661" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B661" s="9" t="s">
         <v>661</v>
       </c>
       <c r="C661" s="10">
-        <v>271</v>
+        <v>21</v>
       </c>
     </row>
     <row r="662" ht="14.25">
@@ -10071,7 +10068,7 @@
         <v>662</v>
       </c>
       <c r="C662" s="10">
-        <v>21</v>
+        <v>40</v>
       </c>
     </row>
     <row r="663" ht="14.25">
@@ -10082,7 +10079,7 @@
         <v>663</v>
       </c>
       <c r="C663" s="10">
-        <v>40</v>
+        <v>25</v>
       </c>
     </row>
     <row r="664" ht="14.25">
@@ -10093,29 +10090,29 @@
         <v>664</v>
       </c>
       <c r="C664" s="10">
-        <v>25</v>
+        <v>35</v>
       </c>
     </row>
     <row r="665" ht="14.25">
       <c r="A665" s="1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B665" s="9" t="s">
         <v>665</v>
       </c>
       <c r="C665" s="10">
-        <v>35</v>
+        <v>186</v>
       </c>
     </row>
     <row r="666" ht="14.25">
       <c r="A666" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B666" s="9" t="s">
         <v>666</v>
       </c>
       <c r="C666" s="10">
-        <v>186</v>
+        <v>40</v>
       </c>
     </row>
     <row r="667" ht="14.25">
@@ -10123,7 +10120,7 @@
         <v>3</v>
       </c>
       <c r="B667" s="9" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="C667" s="10">
         <v>40</v>
@@ -10137,7 +10134,7 @@
         <v>667</v>
       </c>
       <c r="C668" s="10">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="669" ht="14.25">
@@ -10148,7 +10145,7 @@
         <v>668</v>
       </c>
       <c r="C669" s="10">
-        <v>38</v>
+        <v>6</v>
       </c>
     </row>
     <row r="670" ht="14.25">
@@ -10170,7 +10167,7 @@
         <v>670</v>
       </c>
       <c r="C671" s="10">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="672" ht="14.25">
@@ -10181,7 +10178,7 @@
         <v>671</v>
       </c>
       <c r="C672" s="10">
-        <v>9</v>
+        <v>30</v>
       </c>
     </row>
     <row r="673" ht="14.25">
@@ -10192,7 +10189,7 @@
         <v>672</v>
       </c>
       <c r="C673" s="10">
-        <v>30</v>
+        <v>65</v>
       </c>
     </row>
     <row r="674" ht="14.25">
@@ -10203,7 +10200,7 @@
         <v>673</v>
       </c>
       <c r="C674" s="10">
-        <v>65</v>
+        <v>38</v>
       </c>
     </row>
     <row r="675" ht="14.25">
@@ -10211,10 +10208,10 @@
         <v>3</v>
       </c>
       <c r="B675" s="9" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="C675" s="10">
-        <v>38</v>
+        <v>29</v>
       </c>
     </row>
     <row r="676" ht="14.25">
@@ -10225,7 +10222,7 @@
         <v>674</v>
       </c>
       <c r="C676" s="10">
-        <v>29</v>
+        <v>38</v>
       </c>
     </row>
     <row r="677" ht="14.25">
@@ -10233,10 +10230,10 @@
         <v>3</v>
       </c>
       <c r="B677" s="9" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="C677" s="10">
-        <v>38</v>
+        <v>29</v>
       </c>
     </row>
     <row r="678" ht="14.25">
@@ -10247,7 +10244,7 @@
         <v>675</v>
       </c>
       <c r="C678" s="10">
-        <v>29</v>
+        <v>45</v>
       </c>
     </row>
     <row r="679" ht="14.25">
@@ -10258,7 +10255,7 @@
         <v>676</v>
       </c>
       <c r="C679" s="10">
-        <v>45</v>
+        <v>35</v>
       </c>
     </row>
     <row r="680" ht="14.25">
@@ -10269,7 +10266,7 @@
         <v>677</v>
       </c>
       <c r="C680" s="10">
-        <v>35</v>
+        <v>140</v>
       </c>
     </row>
     <row r="681" ht="14.25">
@@ -10280,7 +10277,7 @@
         <v>678</v>
       </c>
       <c r="C681" s="10">
-        <v>140</v>
+        <v>4</v>
       </c>
     </row>
     <row r="682" ht="14.25">
@@ -10291,7 +10288,7 @@
         <v>679</v>
       </c>
       <c r="C682" s="10">
-        <v>4</v>
+        <v>85</v>
       </c>
     </row>
     <row r="683" ht="14.25">
@@ -10302,7 +10299,7 @@
         <v>680</v>
       </c>
       <c r="C683" s="10">
-        <v>85</v>
+        <v>5</v>
       </c>
     </row>
     <row r="684" ht="14.25">
@@ -10313,29 +10310,29 @@
         <v>681</v>
       </c>
       <c r="C684" s="10">
-        <v>5</v>
+        <v>29</v>
       </c>
     </row>
     <row r="685" ht="14.25">
       <c r="A685" s="1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B685" s="9" t="s">
         <v>682</v>
       </c>
       <c r="C685" s="10">
-        <v>29</v>
+        <v>226</v>
       </c>
     </row>
     <row r="686" ht="14.25">
       <c r="A686" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B686" s="9" t="s">
         <v>683</v>
       </c>
       <c r="C686" s="10">
-        <v>226</v>
+        <v>2.5899999999999999</v>
       </c>
     </row>
     <row r="687" ht="14.25">
@@ -10346,7 +10343,7 @@
         <v>684</v>
       </c>
       <c r="C687" s="10">
-        <v>2.5899999999999999</v>
+        <v>66</v>
       </c>
     </row>
     <row r="688" ht="14.25">
@@ -10357,7 +10354,7 @@
         <v>685</v>
       </c>
       <c r="C688" s="10">
-        <v>66</v>
+        <v>106</v>
       </c>
     </row>
     <row r="689" ht="14.25">
@@ -10368,7 +10365,7 @@
         <v>686</v>
       </c>
       <c r="C689" s="10">
-        <v>106</v>
+        <v>86</v>
       </c>
     </row>
     <row r="690" ht="14.25">
@@ -10379,7 +10376,7 @@
         <v>687</v>
       </c>
       <c r="C690" s="10">
-        <v>86</v>
+        <v>126</v>
       </c>
     </row>
     <row r="691" ht="14.25">
@@ -10390,7 +10387,7 @@
         <v>688</v>
       </c>
       <c r="C691" s="10">
-        <v>126</v>
+        <v>66</v>
       </c>
     </row>
     <row r="692" ht="14.25">
@@ -10401,7 +10398,7 @@
         <v>689</v>
       </c>
       <c r="C692" s="10">
-        <v>66</v>
+        <v>106</v>
       </c>
     </row>
     <row r="693" ht="14.25">
@@ -10412,7 +10409,7 @@
         <v>690</v>
       </c>
       <c r="C693" s="10">
-        <v>106</v>
+        <v>66</v>
       </c>
     </row>
     <row r="694" ht="14.25">
@@ -10423,7 +10420,7 @@
         <v>691</v>
       </c>
       <c r="C694" s="10">
-        <v>66</v>
+        <v>106</v>
       </c>
     </row>
     <row r="695" ht="14.25">
@@ -10434,7 +10431,7 @@
         <v>692</v>
       </c>
       <c r="C695" s="10">
-        <v>106</v>
+        <v>66</v>
       </c>
     </row>
     <row r="696" ht="14.25">
@@ -10456,7 +10453,7 @@
         <v>694</v>
       </c>
       <c r="C697" s="10">
-        <v>66</v>
+        <v>106</v>
       </c>
     </row>
     <row r="698" ht="14.25">
@@ -10467,7 +10464,7 @@
         <v>695</v>
       </c>
       <c r="C698" s="10">
-        <v>106</v>
+        <v>66</v>
       </c>
     </row>
     <row r="699" ht="14.25">
@@ -10478,7 +10475,7 @@
         <v>696</v>
       </c>
       <c r="C699" s="10">
-        <v>66</v>
+        <v>106</v>
       </c>
     </row>
     <row r="700" ht="14.25">
@@ -10489,7 +10486,7 @@
         <v>697</v>
       </c>
       <c r="C700" s="10">
-        <v>106</v>
+        <v>66</v>
       </c>
     </row>
     <row r="701" ht="14.25">
@@ -10500,29 +10497,29 @@
         <v>698</v>
       </c>
       <c r="C701" s="10">
-        <v>66</v>
+        <v>106</v>
       </c>
     </row>
     <row r="702" ht="14.25">
       <c r="A702" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B702" s="9" t="s">
+      <c r="B702" s="11" t="s">
         <v>699</v>
       </c>
-      <c r="C702" s="10">
-        <v>106</v>
+      <c r="C702" s="3">
+        <v>100</v>
       </c>
     </row>
     <row r="703" ht="14.25">
       <c r="A703" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B703" s="11" t="s">
+      <c r="B703" s="9" t="s">
         <v>700</v>
       </c>
-      <c r="C703" s="3">
-        <v>100</v>
+      <c r="C703" s="10">
+        <v>66</v>
       </c>
     </row>
     <row r="704" ht="14.25">
@@ -10533,7 +10530,7 @@
         <v>701</v>
       </c>
       <c r="C704" s="10">
-        <v>66</v>
+        <v>106</v>
       </c>
     </row>
     <row r="705" ht="14.25">
@@ -10544,7 +10541,7 @@
         <v>702</v>
       </c>
       <c r="C705" s="10">
-        <v>106</v>
+        <v>85</v>
       </c>
     </row>
     <row r="706" ht="14.25">
@@ -10566,7 +10563,7 @@
         <v>704</v>
       </c>
       <c r="C707" s="10">
-        <v>85</v>
+        <v>78</v>
       </c>
     </row>
     <row r="708" ht="14.25">
@@ -10577,7 +10574,7 @@
         <v>705</v>
       </c>
       <c r="C708" s="10">
-        <v>78</v>
+        <v>10</v>
       </c>
     </row>
     <row r="709" ht="14.25">
@@ -10588,7 +10585,7 @@
         <v>706</v>
       </c>
       <c r="C709" s="10">
-        <v>10</v>
+        <v>100</v>
       </c>
     </row>
     <row r="710" ht="14.25">
@@ -10599,7 +10596,7 @@
         <v>707</v>
       </c>
       <c r="C710" s="10">
-        <v>100</v>
+        <v>25</v>
       </c>
     </row>
     <row r="711" ht="14.25">
@@ -10610,7 +10607,7 @@
         <v>708</v>
       </c>
       <c r="C711" s="10">
-        <v>25</v>
+        <v>147.5</v>
       </c>
     </row>
     <row r="712" ht="14.25">
@@ -10621,7 +10618,7 @@
         <v>709</v>
       </c>
       <c r="C712" s="10">
-        <v>147.5</v>
+        <v>32</v>
       </c>
     </row>
     <row r="713" ht="14.25">
@@ -10632,7 +10629,7 @@
         <v>710</v>
       </c>
       <c r="C713" s="10">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="714" ht="14.25">
@@ -10643,7 +10640,7 @@
         <v>711</v>
       </c>
       <c r="C714" s="10">
-        <v>30</v>
+        <v>50</v>
       </c>
     </row>
     <row r="715" ht="14.25">
@@ -10654,7 +10651,7 @@
         <v>712</v>
       </c>
       <c r="C715" s="10">
-        <v>50</v>
+        <v>43</v>
       </c>
     </row>
     <row r="716" ht="14.25">
@@ -10665,7 +10662,7 @@
         <v>713</v>
       </c>
       <c r="C716" s="10">
-        <v>43</v>
+        <v>15</v>
       </c>
     </row>
     <row r="717" ht="14.25">
@@ -10676,7 +10673,7 @@
         <v>714</v>
       </c>
       <c r="C717" s="10">
-        <v>15</v>
+        <v>80</v>
       </c>
     </row>
     <row r="718" ht="14.25">
@@ -10687,7 +10684,7 @@
         <v>715</v>
       </c>
       <c r="C718" s="10">
-        <v>80</v>
+        <v>3</v>
       </c>
     </row>
     <row r="719" ht="14.25">
@@ -10698,7 +10695,7 @@
         <v>716</v>
       </c>
       <c r="C719" s="10">
-        <v>3</v>
+        <v>23</v>
       </c>
     </row>
     <row r="720" ht="14.25">
@@ -10709,19 +10706,13 @@
         <v>717</v>
       </c>
       <c r="C720" s="10">
-        <v>23</v>
+        <v>57</v>
       </c>
     </row>
     <row r="721" ht="14.25">
-      <c r="A721" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B721" s="9" t="s">
-        <v>718</v>
-      </c>
-      <c r="C721" s="10">
-        <v>57</v>
-      </c>
+      <c r="A721" s="1"/>
+      <c r="B721" s="2"/>
+      <c r="C721" s="3"/>
     </row>
     <row r="722" ht="14.25">
       <c r="A722" s="1"/>
@@ -11233,14 +11224,9 @@
       <c r="B823" s="2"/>
       <c r="C823" s="3"/>
     </row>
-    <row r="824" ht="14.25">
-      <c r="A824" s="1"/>
-      <c r="B824" s="2"/>
-      <c r="C824" s="3"/>
-    </row>
   </sheetData>
-  <sortState ref="A2:C721" columnSort="0">
-    <sortCondition sortBy="value" descending="0" ref="B2:B721"/>
+  <sortState ref="A2:C720" columnSort="0">
+    <sortCondition sortBy="value" descending="0" ref="B2:B720"/>
   </sortState>
   <printOptions headings="0" gridLines="0"/>
   <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>

</xml_diff>

<commit_message>
ATUALIZAÇÃO TABELA DE PREÇOS
</commit_message>
<xml_diff>
--- a/orcamento/valores_exames_samvida.xlsx
+++ b/orcamento/valores_exames_samvida.xlsx
@@ -699,7 +699,7 @@
     <t xml:space="preserve">IgE ESPECIFICO (E5) - Epitélios - CASPA/PELO DE CAO</t>
   </si>
   <si>
-    <t xml:space="preserve">IgE ESPECIFICO (E82) - Epitélios - PÊLO DE COELHO</t>
+    <t xml:space="preserve">IgE ESPECIFICO (E82) - Epitélios - PELO DE COELHO</t>
   </si>
   <si>
     <t xml:space="preserve">IgE ESPECIFICO (F1) - Alimentos - CLARA DE OVO</t>
@@ -771,7 +771,7 @@
     <t xml:space="preserve">IgE ESPECIFICO (I4) - Venenos - MARIMBONDO</t>
   </si>
   <si>
-    <t xml:space="preserve">IgE ESPECIFICO (K70) - Ocupacionais - GRÃO DE CAFÉ</t>
+    <t xml:space="preserve">IgE ESPECIFICO (K70) - Ocupacionais - GRAO DE CAFE</t>
   </si>
   <si>
     <t xml:space="preserve">IgE PAINEL (FX1) - OLEAGENOSAS</t>
@@ -885,16 +885,16 @@
     <t xml:space="preserve">PARASITOLOGICO - COLETA COM MIF</t>
   </si>
   <si>
-    <t xml:space="preserve">PARASITOLÓGICO 1ª AMOSTRA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PARASITOLÓGICO 2ª AMOSTRA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PARASITOLÓGICO 3ª AMOSTRA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PARASITOLÓGICO DE FEZES</t>
+    <t xml:space="preserve">PARASITOLOGICO 1ª AMOSTRA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PARASITOLOGICO 2ª AMOSTRA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PARASITOLOGICO 3ª AMOSTRA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PARASITOLOGICO DE FEZES</t>
   </si>
   <si>
     <t xml:space="preserve">PARATORMONIO - Molecula intacta</t>
@@ -1272,7 +1272,7 @@
     <t xml:space="preserve">RM PERNA E C/CONTRASTE</t>
   </si>
   <si>
-    <t xml:space="preserve">RM PESCOCO</t>
+    <t xml:space="preserve">RM PESCOÇO</t>
   </si>
   <si>
     <t xml:space="preserve">RM PESCOÇO C/CONTRASTE</t>
@@ -1383,13 +1383,13 @@
     <t xml:space="preserve">RM VIAS BILIARES</t>
   </si>
   <si>
-    <t xml:space="preserve">ROTAVÍRUS - Pesquisa</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RUBÉOLA - Anticorpos IgG</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RUBÉOLA - Anticorpos IgM</t>
+    <t xml:space="preserve">ROTAVIRUS - Pesquisa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RUBEOLA - Anticorpos IgG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RUBEOLA - Anticorpos IgM</t>
   </si>
   <si>
     <t xml:space="preserve">RX ABDOME AGUDO</t>
@@ -1611,7 +1611,7 @@
     <t xml:space="preserve">RX PERNA E</t>
   </si>
   <si>
-    <t xml:space="preserve">RX PESCOCO</t>
+    <t xml:space="preserve">RX PESCOÇO</t>
   </si>
   <si>
     <t xml:space="preserve">RX PUNHO D</t>
@@ -1620,10 +1620,10 @@
     <t xml:space="preserve">RX PUNHO E</t>
   </si>
   <si>
-    <t xml:space="preserve">RX PÉ D</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RX PÉ E</t>
+    <t xml:space="preserve">RX PE D</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RX PE E</t>
   </si>
   <si>
     <t xml:space="preserve">RX SACRO COCCIX</t>
@@ -1668,7 +1668,7 @@
     <t xml:space="preserve">SARAMPO - Anticorpos IgM</t>
   </si>
   <si>
-    <t xml:space="preserve">SELÊNIO SÉRICO</t>
+    <t xml:space="preserve">SELENIO SERICO</t>
   </si>
   <si>
     <t>SEROTONINA</t>
@@ -1680,19 +1680,19 @@
     <t xml:space="preserve">SULFATO DE DEHIDROPIANDROSTERONA</t>
   </si>
   <si>
-    <t xml:space="preserve">SUMÁRIO DE URINA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SÍFILIS - VDRL</t>
-  </si>
-  <si>
-    <t>SÓDIO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SÓDIO URINÁRIO - 24h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SÓDIO URINÁRIO - AMOSTRA ISOLADA</t>
+    <t xml:space="preserve">SUMARIO DE URINA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SIFILIS - VDRL</t>
+  </si>
+  <si>
+    <t>SODIO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SODIO URINARIO - 24h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SODIO URINARIO - AMOSTRA ISOLADA</t>
   </si>
   <si>
     <t xml:space="preserve">T3 - TRIIODOTIRONINA</t>
@@ -1737,13 +1737,13 @@
     <t xml:space="preserve">TC ARTICULACOES TEMPOROMANDIBULARES BILATERAL</t>
   </si>
   <si>
-    <t xml:space="preserve">TC ARTICULAÇÃO EXTERNO CLAVICULAR D</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TC ARTICULAÇÃO EXTERNO CLAVICULAR E</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TC ARTICULAÇÕES MEMBROS INFERIORES</t>
+    <t xml:space="preserve">TC ARTICULAÇAO EXTERNO CLAVICULAR D</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TC ARTICULAÇAO EXTERNO CLAVICULAR E</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TC ARTICULAÇOES MEMBROS INFERIORES</t>
   </si>
   <si>
     <t xml:space="preserve">TC BRACO D</t>
@@ -1827,10 +1827,10 @@
     <t xml:space="preserve">TC FACE C/ CONTRASTE</t>
   </si>
   <si>
-    <t xml:space="preserve">TC HIPÓFISE C/CONTRASTE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TC HIPÓFISE S/CONTRASTE</t>
+    <t xml:space="preserve">TC HIPOFISE C/CONTRASTE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TC HIPOFISE S/CONTRASTE</t>
   </si>
   <si>
     <t xml:space="preserve">TC JOELHO D</t>
@@ -2007,10 +2007,10 @@
     <t xml:space="preserve">TEMPO DE TROMBOPLASTINA PARCIAL ATIVADA</t>
   </si>
   <si>
-    <t xml:space="preserve">TESTE DE TOLERÂNCIA A GLICOSE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TESTE ERGOMÉTRICO</t>
+    <t xml:space="preserve">TESTE DE TOLERANCIA A GLICOSE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TESTE ERGOMETRICO</t>
   </si>
   <si>
     <t xml:space="preserve">TESTOSTERONA LIVRE</t>
@@ -2049,7 +2049,7 @@
     <t xml:space="preserve">TRIAGEM TOXICOLOGICA</t>
   </si>
   <si>
-    <t>TRIGLICERÍDEOS</t>
+    <t>TRIGLICERIDEOS</t>
   </si>
   <si>
     <t xml:space="preserve">TROPONINA CARDIACA - T</t>
@@ -2064,7 +2064,7 @@
     <t xml:space="preserve">UROGRAFIA EXCRETORA</t>
   </si>
   <si>
-    <t xml:space="preserve">URÉIA URINÁRIA - 24h</t>
+    <t xml:space="preserve">UREIA URINARIA - 24h</t>
   </si>
   <si>
     <t xml:space="preserve">USG ABDOME SUPERIOR</t>
@@ -2085,10 +2085,10 @@
     <t xml:space="preserve">USG AXILAS DOPPLER</t>
   </si>
   <si>
-    <t xml:space="preserve">USG ENDOVAGINAL + PÉLVICA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">USG ENDOVAGINAL + PÉLVICA DOPPLER</t>
+    <t xml:space="preserve">USG ENDOVAGINAL + PELVICA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">USG ENDOVAGINAL + PELVICA DOPPLER</t>
   </si>
   <si>
     <t xml:space="preserve">USG GESTACIONAL</t>
@@ -2106,19 +2106,19 @@
     <t xml:space="preserve">USG PROSTATA TRANS ABD DOPPLER</t>
   </si>
   <si>
-    <t xml:space="preserve">USG PÉLVICA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">USG PÉLVICA DOPPLER</t>
+    <t xml:space="preserve">USG PELVICA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">USG PELVICA DOPPLER</t>
   </si>
   <si>
     <t xml:space="preserve">USG TIREOIDE</t>
   </si>
   <si>
-    <t xml:space="preserve">USG VIAS URINÁRIAS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">USG VIAS URINÁRIAS DOPPLER</t>
+    <t xml:space="preserve">USG VIAS URINARIAS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">USG VIAS URINARIAS DOPPLER</t>
   </si>
   <si>
     <t xml:space="preserve">VARICELA ZOSTER - Anticorpos IgG</t>
@@ -2127,7 +2127,7 @@
     <t xml:space="preserve">VARICELA ZOSTER - Anticorpos IgM</t>
   </si>
   <si>
-    <t xml:space="preserve">VASOPRESSINA - antidiurético - AD</t>
+    <t xml:space="preserve">VASOPRESSINA - antidiuretico - AD</t>
   </si>
   <si>
     <t xml:space="preserve">VELOCIDADE DE HEMOSSEDIMENTACAO - VHS</t>
@@ -2151,22 +2151,22 @@
     <t xml:space="preserve">VITAMINA E</t>
   </si>
   <si>
-    <t xml:space="preserve">ZINCO SÉRICO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ÁCIDO LÁTICO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ÁCIDO VANIL MANDELICO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ÁCIDO ÚRICO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ÍNDICE DE SATURAÇÃO DA TRANSFERRINA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ÍNDICE TIROXINA LIVRE</t>
+    <t xml:space="preserve">ZINCO SERICO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ACIDO LATICO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ACIDO VANIL MANDELICO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ACIDO URICO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">INDICE DE SATURAÇÃO DA TRANSFERRINA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">INDICE TIROXINA LIVRE</t>
   </si>
 </sst>
 </file>
@@ -2778,7 +2778,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetViews>
-    <sheetView topLeftCell="A289" zoomScale="100" workbookViewId="0">
+    <sheetView topLeftCell="A168" zoomScale="100" workbookViewId="0">
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>

</xml_diff>